<commit_message>
added ckeditor for rich text
</commit_message>
<xml_diff>
--- a/Blog_Project/TestUnitarios.xlsx
+++ b/Blog_Project/TestUnitarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo_GitHub\Proyecto_Final_GimenoAndres\Proyecto_Final_GimenoAndres\Blog_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410ABDE5-E46C-41D5-BA2B-14A4AA8D1D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6366C29-48F5-46FB-A940-0CEAB8F22DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6225" yWindow="2790" windowWidth="21600" windowHeight="11295" xr2:uid="{8DC43982-73BF-4F4F-AD0D-12F501BCA782}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Muestra detalles al usuario logeado</t>
+  </si>
+  <si>
+    <t>Datos que superen las condiciones del form</t>
+  </si>
+  <si>
+    <t>El programa deberia alojar un error de superacion de caracteres.</t>
+  </si>
+  <si>
+    <t>El error es mostrado</t>
   </si>
 </sst>
 </file>
@@ -548,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872B1C44-31D4-41C2-AF15-3BC99982C5DD}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,6 +824,26 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44956</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D2:D3"/>

</xml_diff>